<commit_message>
bug fix: color orange duplicates
</commit_message>
<xml_diff>
--- a/src/pages/data/Datos.xlsx
+++ b/src/pages/data/Datos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="225">
   <si>
     <t>First Name</t>
   </si>
@@ -70,7 +70,7 @@
     <t>MI</t>
   </si>
   <si>
-    <t>christ.huert21a39172</t>
+    <t>Q68360-88519</t>
   </si>
   <si>
     <t>q9h9*!PuwO</t>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>varughese.kris408@yahoo.com</t>
-  </si>
-  <si>
-    <t>Q68360-88519</t>
   </si>
   <si>
     <t>John</t>
@@ -904,8 +901,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="bottom"/>
@@ -1321,7 +1318,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
@@ -1337,43 +1334,43 @@
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="C4" s="18">
         <v>25302</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="19">
         <v>253</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="L4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="15"/>
@@ -1390,46 +1387,46 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="18">
         <v>19225</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>46</v>
       </c>
       <c r="F5" s="19">
         <v>812</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="K5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
@@ -1445,19 +1442,19 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="C6" s="18">
         <v>24391</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="F6" s="19">
         <v>641</v>
@@ -1472,16 +1469,16 @@
         <v>29</v>
       </c>
       <c r="J6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="15"/>
@@ -1498,46 +1495,46 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="C7" s="18">
         <v>29287</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="F7" s="19">
         <v>814</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="K7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="L7" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" s="17" t="s">
+      <c r="N7" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>67</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
@@ -1553,46 +1550,46 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C8" s="18">
         <v>19819</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="F8" s="19">
         <v>651</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="L8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="17" t="s">
+      <c r="N8" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
@@ -1608,43 +1605,43 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="C9" s="18">
         <v>30760</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="F9" s="19">
         <v>295</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>83</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="15"/>
@@ -1661,43 +1658,43 @@
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="C10" s="18">
         <v>22868</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>87</v>
       </c>
       <c r="F10" s="19">
         <v>529</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="K10" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="L10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="15"/>
@@ -1714,43 +1711,43 @@
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C11" s="18">
         <v>33755</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="F11" s="19">
         <v>164</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I11" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="L11" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>99</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="15"/>
@@ -1767,43 +1764,43 @@
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="C12" s="18">
         <v>22238</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="F12" s="19">
         <v>874</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="K12" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="L12" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>108</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="15"/>
@@ -1820,43 +1817,43 @@
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>110</v>
       </c>
       <c r="C13" s="22">
         <v>18533</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="F13" s="23">
         <v>557</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H13" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="K13" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="L13" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>116</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -1873,43 +1870,43 @@
     </row>
     <row r="14" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>118</v>
       </c>
       <c r="C14" s="26">
         <v>34730</v>
       </c>
       <c r="D14" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="F14" s="27">
         <v>522</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="K14" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="L14" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -1926,43 +1923,43 @@
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>125</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>126</v>
       </c>
       <c r="C15" s="22">
         <v>25419</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="F15" s="23">
         <v>217</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J15" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="K15" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="L15" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="M15" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>132</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -1979,43 +1976,43 @@
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="26">
         <v>28973</v>
       </c>
       <c r="D16" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>134</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>135</v>
       </c>
       <c r="F16" s="27">
         <v>156</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I16" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="K16" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="L16" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="M16" s="25" t="s">
         <v>138</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="M16" s="25" t="s">
-        <v>139</v>
       </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -2032,43 +2029,43 @@
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>140</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>141</v>
       </c>
       <c r="C17" s="26">
         <v>29989</v>
       </c>
       <c r="D17" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>142</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>143</v>
       </c>
       <c r="F17" s="27">
         <v>499</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I17" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="K17" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="L17" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="M17" s="25" t="s">
         <v>146</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>147</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2085,43 +2082,43 @@
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>148</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="C18" s="22">
         <v>20751</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>150</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>151</v>
       </c>
       <c r="F18" s="23">
         <v>412</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I18" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="K18" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="L18" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="M18" s="21" t="s">
         <v>154</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>155</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -2138,43 +2135,43 @@
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>157</v>
       </c>
       <c r="C19" s="26">
         <v>31548</v>
       </c>
       <c r="D19" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>158</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>159</v>
       </c>
       <c r="F19" s="27">
         <v>603</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I19" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="J19" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="K19" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="L19" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="M19" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>163</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
@@ -2191,43 +2188,43 @@
     </row>
     <row r="20" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>165</v>
       </c>
       <c r="C20" s="22">
         <v>30398</v>
       </c>
       <c r="D20" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>167</v>
       </c>
       <c r="F20" s="23">
         <v>935</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I20" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="J20" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="K20" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="L20" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="M20" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>171</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -2244,43 +2241,43 @@
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>172</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>173</v>
       </c>
       <c r="C21" s="26">
         <v>26305</v>
       </c>
       <c r="D21" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>174</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>175</v>
       </c>
       <c r="F21" s="27">
         <v>861</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I21" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J21" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="K21" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="L21" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="M21" s="25" t="s">
         <v>178</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>179</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -2297,43 +2294,43 @@
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>181</v>
       </c>
       <c r="C22" s="22">
         <v>21956</v>
       </c>
       <c r="D22" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>182</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>183</v>
       </c>
       <c r="F22" s="23">
         <v>947</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J22" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="K22" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="L22" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="M22" s="21" t="s">
         <v>185</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="M22" s="21" t="s">
-        <v>186</v>
       </c>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -2350,19 +2347,19 @@
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>188</v>
       </c>
       <c r="C23" s="26">
         <v>24146</v>
       </c>
       <c r="D23" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="F23" s="27">
         <v>123</v>
@@ -2374,19 +2371,19 @@
         <v>28</v>
       </c>
       <c r="I23" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="K23" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="K23" s="25" t="s">
+      <c r="L23" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="M23" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>194</v>
       </c>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -2403,43 +2400,43 @@
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>196</v>
       </c>
       <c r="C24" s="22">
         <v>23221</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="F24" s="23">
         <v>936</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="J24" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="K24" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="L24" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="M24" s="21" t="s">
         <v>201</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>202</v>
       </c>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
@@ -2456,43 +2453,43 @@
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>203</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>204</v>
       </c>
       <c r="C25" s="26">
         <v>33638</v>
       </c>
       <c r="D25" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>205</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>206</v>
       </c>
       <c r="F25" s="27">
         <v>482</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="K25" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="K25" s="25" t="s">
+      <c r="L25" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="M25" s="25" t="s">
         <v>208</v>
-      </c>
-      <c r="L25" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>209</v>
       </c>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
@@ -2509,43 +2506,43 @@
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>210</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>211</v>
       </c>
       <c r="C26" s="22">
         <v>26113</v>
       </c>
       <c r="D26" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="F26" s="23">
         <v>316</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H26" s="21" t="s">
         <v>28</v>
       </c>
       <c r="I26" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="J26" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="K26" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="L26" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="M26" s="21" t="s">
         <v>216</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="M26" s="21" t="s">
-        <v>217</v>
       </c>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
@@ -2562,43 +2559,43 @@
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>218</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>219</v>
       </c>
       <c r="C27" s="26">
         <v>28022</v>
       </c>
       <c r="D27" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>220</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>221</v>
       </c>
       <c r="F27" s="27">
         <v>782</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="25" t="s">
         <v>28</v>
       </c>
       <c r="I27" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J27" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="K27" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="K27" s="25" t="s">
+      <c r="L27" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="M27" s="25" t="s">
         <v>224</v>
-      </c>
-      <c r="L27" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>225</v>
       </c>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>

</xml_diff>

<commit_message>
bug fix: duplicado selector fix range, bug fix: exito case delete selector
</commit_message>
<xml_diff>
--- a/src/pages/data/Datos.xlsx
+++ b/src/pages/data/Datos.xlsx
@@ -3,6 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="24000"/>
+  </bookViews>
   <sheets>
     <sheet sheetId="1" name="Hoja 1" state="visible" r:id="rId4"/>
   </sheets>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="224">
   <si>
     <t>First Name</t>
   </si>
@@ -52,6 +55,9 @@
     <t>email address</t>
   </si>
   <si>
+    <t>Application ID</t>
+  </si>
+  <si>
     <t>christina</t>
   </si>
   <si>
@@ -79,9 +85,6 @@
     <t>huerta.christina332@outlook.com</t>
   </si>
   <si>
-    <t>Q97426-26865</t>
-  </si>
-  <si>
     <t>Kris</t>
   </si>
   <si>
@@ -163,7 +166,7 @@
     <t>gitty.r09@yahoo.com</t>
   </si>
   <si>
-    <t>Q37266-17383</t>
+    <t>Q55475-09250</t>
   </si>
   <si>
     <t>Silvana</t>
@@ -187,6 +190,9 @@
     <t>silvana.malcaus894@gmail.com</t>
   </si>
   <si>
+    <t>Q75147-75736</t>
+  </si>
+  <si>
     <t>Samuel</t>
   </si>
   <si>
@@ -211,9 +217,6 @@
     <t>sam.quinones61@hotmail.com</t>
   </si>
   <si>
-    <t>Q41595-97201</t>
-  </si>
-  <si>
     <t>Yevgeniy</t>
   </si>
   <si>
@@ -236,9 +239,6 @@
   </si>
   <si>
     <t>yevgeniy.tsvi42@gmail.com</t>
-  </si>
-  <si>
-    <t>Q76529-18789</t>
   </si>
   <si>
     <t>Morgan</t>
@@ -697,7 +697,7 @@
     <numFmt numFmtId="165" formatCode="0000-00-0000"/>
     <numFmt numFmtId="166" formatCode="[$-2540A]mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -730,9 +730,15 @@
     <font>
       <b/>
       <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +760,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -860,92 +877,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,7 +950,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1154,6 +1140,8 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1164,11 +1152,13 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="12.63"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="12.5703125"/>
   <cols>
-    <col min="1" max="6" width="12.63" customWidth="1"/>
+    <col min="1" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -1211,7 +1201,9 @@
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7"/>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
@@ -1225,47 +1217,45 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10">
         <v>26622</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="12">
         <v>604</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="13">
         <v>48420</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="N2" s="16"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
@@ -1317,9 +1307,7 @@
       <c r="M3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="N3" s="16"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
@@ -1372,7 +1360,7 @@
       <c r="M4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="16"/>
+      <c r="N4" s="21"/>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
@@ -1480,7 +1468,9 @@
       <c r="M6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="16"/>
+      <c r="N6" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
@@ -1495,19 +1485,19 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="18">
         <v>29287</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F7" s="19">
         <v>814</v>
@@ -1519,23 +1509,21 @@
         <v>28</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="16" t="s">
         <v>66</v>
       </c>
+      <c r="N7" s="16"/>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
@@ -1588,9 +1576,7 @@
       <c r="M8" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="16" t="s">
-        <v>75</v>
-      </c>
+      <c r="N8" s="16"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
@@ -1605,19 +1591,19 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C9" s="18">
         <v>30760</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="F9" s="19">
         <v>295</v>
@@ -1632,16 +1618,16 @@
         <v>38</v>
       </c>
       <c r="J9" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="L9" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="15"/>
@@ -1658,19 +1644,19 @@
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="C10" s="18">
         <v>22868</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>86</v>
       </c>
       <c r="F10" s="19">
         <v>529</v>
@@ -1682,19 +1668,19 @@
         <v>28</v>
       </c>
       <c r="I10" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="K10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="L10" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="15"/>
@@ -1711,19 +1697,19 @@
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="C11" s="18">
         <v>33755</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="F11" s="19">
         <v>164</v>
@@ -1735,19 +1721,19 @@
         <v>28</v>
       </c>
       <c r="I11" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="K11" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="L11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="15"/>
@@ -1764,43 +1750,43 @@
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="C12" s="18">
         <v>22238</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>102</v>
       </c>
       <c r="F12" s="19">
         <v>874</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="K12" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="L12" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="M12" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>107</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="15"/>
@@ -1816,44 +1802,44 @@
       <c r="Y12" s="15"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="C13" s="23">
+        <v>18533</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="22">
-        <v>18533</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="24">
+        <v>557</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="F13" s="23">
-        <v>557</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="21" t="s">
+      <c r="J13" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="K13" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="L13" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="M13" s="22" t="s">
         <v>114</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>115</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -1869,44 +1855,44 @@
       <c r="Y13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="C14" s="27">
+        <v>34730</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="26">
-        <v>34730</v>
-      </c>
-      <c r="D14" s="25" t="s">
+      <c r="E14" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="F14" s="28">
+        <v>522</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="F14" s="27">
-        <v>522</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="25" t="s">
+      <c r="J14" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="K14" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="L14" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
@@ -1922,44 +1908,44 @@
       <c r="Y14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" s="23">
+        <v>25419</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="22">
-        <v>25419</v>
-      </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="F15" s="24">
+        <v>217</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="23">
-        <v>217</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="21" t="s">
+      <c r="J15" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="K15" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="L15" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="M15" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>131</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
@@ -1975,44 +1961,44 @@
       <c r="Y15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="27">
+        <v>28973</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="26">
-        <v>28973</v>
-      </c>
-      <c r="D16" s="25" t="s">
+      <c r="E16" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="F16" s="28">
+        <v>156</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="27">
-        <v>156</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="25" t="s">
+      <c r="J16" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="K16" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="L16" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="26" t="s">
         <v>137</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="M16" s="25" t="s">
-        <v>138</v>
       </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
@@ -2028,44 +2014,44 @@
       <c r="Y16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="27">
+        <v>29989</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="26">
-        <v>29989</v>
-      </c>
-      <c r="D17" s="25" t="s">
+      <c r="E17" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="F17" s="28">
+        <v>499</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="F17" s="27">
-        <v>499</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="25" t="s">
+      <c r="J17" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="K17" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="L17" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="M17" s="26" t="s">
         <v>145</v>
-      </c>
-      <c r="L17" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
@@ -2081,44 +2067,44 @@
       <c r="Y17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="C18" s="23">
+        <v>20751</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="22">
-        <v>20751</v>
-      </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="24">
+        <v>412</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="23">
-        <v>412</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="21" t="s">
+      <c r="J18" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="K18" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="L18" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M18" s="22" t="s">
         <v>153</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>154</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -2134,44 +2120,44 @@
       <c r="Y18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="C19" s="27">
+        <v>31548</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="26">
-        <v>31548</v>
-      </c>
-      <c r="D19" s="25" t="s">
+      <c r="E19" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="F19" s="28">
+        <v>603</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="F19" s="27">
-        <v>603</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="25" t="s">
+      <c r="J19" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="K19" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="L19" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="M19" s="26" t="s">
         <v>161</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>162</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
@@ -2187,44 +2173,44 @@
       <c r="Y19" s="7"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="C20" s="23">
+        <v>30398</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="22">
-        <v>30398</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="24">
+        <v>935</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="F20" s="23">
-        <v>935</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="21" t="s">
+      <c r="J20" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="K20" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="L20" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="M20" s="22" t="s">
         <v>169</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>170</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
@@ -2240,44 +2226,44 @@
       <c r="Y20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="C21" s="27">
+        <v>26305</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="C21" s="26">
-        <v>26305</v>
-      </c>
-      <c r="D21" s="25" t="s">
+      <c r="E21" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="F21" s="28">
+        <v>861</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="27">
-        <v>861</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="25" t="s">
+      <c r="J21" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="K21" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="L21" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="M21" s="26" t="s">
         <v>177</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>178</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
@@ -2293,44 +2279,44 @@
       <c r="Y21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="C22" s="23">
+        <v>21956</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C22" s="22">
-        <v>21956</v>
-      </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="F22" s="24">
+        <v>947</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="F22" s="23">
-        <v>947</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="J22" s="24" t="s">
+      <c r="K22" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="L22" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="M22" s="22" t="s">
         <v>184</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="M22" s="21" t="s">
-        <v>185</v>
       </c>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -2346,44 +2332,44 @@
       <c r="Y22" s="7"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="27">
+        <v>24146</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="26">
-        <v>24146</v>
-      </c>
-      <c r="D23" s="25" t="s">
+      <c r="E23" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="F23" s="28">
+        <v>123</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="F23" s="27">
-        <v>123</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="25" t="s">
+      <c r="J23" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="K23" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="K23" s="25" t="s">
+      <c r="L23" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="M23" s="26" t="s">
         <v>192</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>193</v>
       </c>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
@@ -2399,44 +2385,44 @@
       <c r="Y23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="C24" s="23">
+        <v>23221</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="C24" s="22">
-        <v>23221</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="F24" s="24">
+        <v>936</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="F24" s="23">
-        <v>936</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="21" t="s">
+      <c r="J24" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="K24" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="L24" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="M24" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>201</v>
       </c>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
@@ -2452,44 +2438,44 @@
       <c r="Y24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="27">
+        <v>33638</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C25" s="26">
-        <v>33638</v>
-      </c>
-      <c r="D25" s="25" t="s">
+      <c r="E25" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="F25" s="28">
+        <v>482</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="F25" s="27">
-        <v>482</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="28" t="s">
+      <c r="K25" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="K25" s="25" t="s">
+      <c r="L25" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="M25" s="26" t="s">
         <v>207</v>
-      </c>
-      <c r="L25" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>208</v>
       </c>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
@@ -2505,44 +2491,44 @@
       <c r="Y25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="C26" s="23">
+        <v>26113</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="C26" s="22">
-        <v>26113</v>
-      </c>
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="F26" s="24">
+        <v>316</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F26" s="23">
-        <v>316</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="21" t="s">
+      <c r="J26" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="K26" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="L26" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="M26" s="22" t="s">
         <v>215</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="M26" s="21" t="s">
-        <v>216</v>
       </c>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
@@ -2558,44 +2544,44 @@
       <c r="Y26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="C27" s="27">
+        <v>28022</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="C27" s="26">
-        <v>28022</v>
-      </c>
-      <c r="D27" s="25" t="s">
+      <c r="E27" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="F27" s="28">
+        <v>782</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="F27" s="27">
-        <v>782</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="25" t="s">
+      <c r="J27" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="K27" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="K27" s="25" t="s">
+      <c r="L27" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="M27" s="26" t="s">
         <v>223</v>
-      </c>
-      <c r="L27" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>224</v>
       </c>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
@@ -3584,5 +3570,6 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>